<commit_message>
S4Loadet fixed 1-to-1 mappings read error. Problem was with the input .xlsx file containing some trailing rows.
</commit_message>
<xml_diff>
--- a/data/S4Loader_configs/s4_to_pdt_one_to_one_mapping.xlsx
+++ b/data/S4Loader_configs/s4_to_pdt_one_to_one_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\work-flix\data\S4Loader_configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\bin\s4loader\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B81ED10-C15E-415B-9D4A-42A866336537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935BE1D2-2D06-40ED-98EF-93762DAFC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="756" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <sheet name="KISK" sheetId="11" r:id="rId11"/>
     <sheet name="LIDE" sheetId="12" r:id="rId12"/>
     <sheet name="LSTN" sheetId="13" r:id="rId13"/>
-    <sheet name="MCCE" sheetId="14" r:id="rId14"/>
+    <sheet name="MCCE" sheetId="30" r:id="rId14"/>
     <sheet name="NETW" sheetId="15" r:id="rId15"/>
     <sheet name="PODE" sheetId="16" r:id="rId16"/>
     <sheet name="PSTN" sheetId="17" r:id="rId17"/>
@@ -5026,18 +5026,18 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:C330"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C4E711-5642-4827-ABA3-DEB4484E578A}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5139,790 +5139,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="1"/>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="1"/>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="1"/>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="1"/>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="1"/>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="1"/>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="1"/>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="1"/>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="1"/>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="1"/>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C111" s="1"/>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C112" s="1"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="1"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="1"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="1"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="1"/>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="1"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="1"/>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C119" s="1"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="1"/>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C121" s="1"/>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="1"/>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C123" s="1"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="1"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="1"/>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C126" s="1"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="1"/>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C128" s="1"/>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C129" s="1"/>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C130" s="1"/>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C131" s="1"/>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="1"/>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C133" s="1"/>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="1"/>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="1"/>
-    </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C136" s="1"/>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C137" s="1"/>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C138" s="1"/>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="1"/>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C140" s="1"/>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C141" s="1"/>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C142" s="1"/>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="1"/>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" s="1"/>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" s="1"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="1"/>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C147" s="1"/>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C148" s="1"/>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C149" s="1"/>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C150" s="1"/>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C152" s="1"/>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C153" s="1"/>
-    </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C154" s="1"/>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C155" s="1"/>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C156" s="1"/>
-    </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C157" s="1"/>
-    </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C158" s="1"/>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C159" s="1"/>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C160" s="1"/>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" s="1"/>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C162" s="1"/>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C163" s="1"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C164" s="1"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="1"/>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C166" s="1"/>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="1"/>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C169" s="1"/>
-    </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C171" s="1"/>
-    </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C172" s="1"/>
-    </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C173" s="1"/>
-    </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C174" s="1"/>
-    </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C175" s="1"/>
-    </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C176" s="1"/>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C177" s="1"/>
-    </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C178" s="1"/>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C179" s="1"/>
-    </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C180" s="1"/>
-    </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C181" s="1"/>
-    </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C182" s="1"/>
-    </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C183" s="1"/>
-    </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C184" s="1"/>
-    </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C185" s="1"/>
-    </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C186" s="1"/>
-    </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C187" s="1"/>
-    </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C188" s="1"/>
-    </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C189" s="1"/>
-    </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C191" s="1"/>
-    </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C192" s="1"/>
-    </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C193" s="1"/>
-    </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C194" s="1"/>
-    </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C195" s="1"/>
-    </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C196" s="1"/>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C197" s="1"/>
-    </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C198" s="1"/>
-    </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C199" s="1"/>
-    </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C200" s="1"/>
-    </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C201" s="1"/>
-    </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C202" s="1"/>
-    </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C203" s="1"/>
-    </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C204" s="1"/>
-    </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C205" s="1"/>
-    </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C206" s="1"/>
-    </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C207" s="1"/>
-    </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C208" s="1"/>
-    </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C209" s="1"/>
-    </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C210" s="1"/>
-    </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C211" s="1"/>
-    </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C212" s="1"/>
-    </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C213" s="1"/>
-    </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C214" s="1"/>
-    </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C215" s="1"/>
-    </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C216" s="1"/>
-    </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C217" s="1"/>
-    </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C218" s="1"/>
-    </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C219" s="1"/>
-    </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C220" s="1"/>
-    </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C221" s="1"/>
-    </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C222" s="1"/>
-    </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C223" s="1"/>
-    </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C224" s="1"/>
-    </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C225" s="1"/>
-    </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C226" s="1"/>
-    </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C227" s="1"/>
-    </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C228" s="1"/>
-    </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C229" s="1"/>
-    </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C230" s="1"/>
-    </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C231" s="1"/>
-    </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C232" s="1"/>
-    </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C233" s="1"/>
-    </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C234" s="1"/>
-    </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C235" s="1"/>
-    </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C236" s="1"/>
-    </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C237" s="1"/>
-    </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C238" s="1"/>
-    </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C239" s="1"/>
-    </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C240" s="1"/>
-    </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C242" s="1"/>
-    </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C243" s="1"/>
-    </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C244" s="1"/>
-    </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C245" s="1"/>
-    </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C246" s="1"/>
-    </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C247" s="1"/>
-    </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C248" s="1"/>
-    </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C249" s="1"/>
-    </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C250" s="1"/>
-    </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C251" s="1"/>
-    </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C252" s="1"/>
-    </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C253" s="1"/>
-    </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C254" s="1"/>
-    </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C255" s="1"/>
-    </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C256" s="1"/>
-    </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C257" s="1"/>
-    </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C258" s="1"/>
-    </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C259" s="1"/>
-    </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C260" s="1"/>
-    </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C261" s="1"/>
-    </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C262" s="1"/>
-    </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C263" s="1"/>
-    </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C265" s="1"/>
-    </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C266" s="1"/>
-    </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C267" s="1"/>
-    </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C268" s="1"/>
-    </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C269" s="1"/>
-    </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C270" s="1"/>
-    </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C271" s="1"/>
-    </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C273" s="1"/>
-    </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C274" s="1"/>
-    </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C275" s="1"/>
-    </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C276" s="1"/>
-    </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C277" s="1"/>
-    </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C278" s="1"/>
-    </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C280" s="1"/>
-    </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C281" s="1"/>
-    </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C282" s="1"/>
-    </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C283" s="1"/>
-    </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C284" s="1"/>
-    </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C285" s="1"/>
-    </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C286" s="1"/>
-    </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C288" s="1"/>
-    </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C289" s="1"/>
-    </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C290" s="1"/>
-    </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C291" s="1"/>
-    </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C292" s="1"/>
-    </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C293" s="1"/>
-    </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C294" s="1"/>
-    </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C296" s="1"/>
-    </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C297" s="1"/>
-    </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C298" s="1"/>
-    </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C299" s="1"/>
-    </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C300" s="1"/>
-    </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C301" s="1"/>
-    </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C302" s="1"/>
-    </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C303" s="1"/>
-    </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C322" s="1"/>
-    </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C323" s="1"/>
-    </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C324" s="1"/>
-    </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C326" s="1"/>
-    </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C327" s="1"/>
-    </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C328" s="1"/>
-    </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C329" s="1"/>
-    </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C330" s="1"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5930,7 +5148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>